<commit_message>
Code For CreatecategoryProduct and Customer
</commit_message>
<xml_diff>
--- a/Discount_TestData.xlsx
+++ b/Discount_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Discount" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Order" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -303,20 +304,20 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.27037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.9"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="14.8962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,7 +396,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -410,23 +411,23 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="9" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1017" style="0" width="9.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.36"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="1016" min="9" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="1021" min="1017" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,7 +490,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -504,19 +505,19 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C1 E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.72"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.3777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="14.0148148148148"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,7 +561,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -575,24 +576,24 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="11" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.53"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.3777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.68518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1020" min="11" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="1022" min="1021" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -720,7 +721,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Discount Test is completed and Tested
</commit_message>
<xml_diff>
--- a/Discount_TestData.xlsx
+++ b/Discount_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Discount" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,6 @@
     <sheet name="Order" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -134,10 +133,19 @@
     <t xml:space="preserve">Customer4</t>
   </si>
   <si>
+    <t xml:space="preserve">Tiered Discount - Tiered Discount:USAGE_BASED</t>
+  </si>
+  <si>
     <t xml:space="preserve">US$45.00</t>
   </si>
   <si>
-    <t xml:space="preserve">US$5.00</t>
+    <t xml:space="preserve">US$49.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please provide Discountable Item / Order and Discount on the Discount Line.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiered Discount% - Tiered Discount%:USAGE_BASED</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
@@ -146,19 +154,67 @@
     <t xml:space="preserve">US$53.00</t>
   </si>
   <si>
-    <t xml:space="preserve">US$16.98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$7.00</t>
+    <t xml:space="preserve">US$59.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(US$43.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(US$58.3)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Volume Discount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Volume Discount:USAGE_BASED</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">US$79.00</t>
   </si>
   <si>
-    <t xml:space="preserve">US$41.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$21.00</t>
+    <t xml:space="preserve">US$97.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$59.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$95.90</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Volume Discount%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Volume Discount%:USAGE_BASED</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">15</t>
@@ -167,19 +223,25 @@
     <t xml:space="preserve">US$93.00</t>
   </si>
   <si>
-    <t xml:space="preserve">US$117.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$57.00</t>
+    <t xml:space="preserve">US$144.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$33.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$138.30</t>
   </si>
   <si>
     <t xml:space="preserve">US$38.00</t>
   </si>
   <si>
-    <t xml:space="preserve">US$142.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$62.00</t>
+    <t xml:space="preserve">US$93.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(US$42.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$85.80</t>
   </si>
 </sst>
 </file>
@@ -190,7 +252,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -221,6 +283,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -264,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -282,6 +350,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,20 +376,20 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.27037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.9"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="14.8962962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="14.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,7 +468,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -411,23 +483,23 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="1016" min="9" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="1021" min="1017" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.52592592592593"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="9" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1017" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,7 +562,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -505,19 +577,19 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="14.0148148148148"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,7 +633,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -574,26 +646,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.68518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="1020" min="11" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="1022" min="1021" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.62222222222222"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="47.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="48.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="14" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="14.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -612,20 +686,29 @@
       <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>36</v>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -635,84 +718,94 @@
       <c r="E2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="I2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="2"/>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +814,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Set the Correct Data for the volume discount amount
</commit_message>
<xml_diff>
--- a/Discount_TestData.xlsx
+++ b/Discount_TestData.xlsx
@@ -157,31 +157,13 @@
     <t xml:space="preserve">US$59.30</t>
   </si>
   <si>
-    <t xml:space="preserve">(US$43.02)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(US$58.3)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Volume Discount</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Volume Discount:USAGE_BASED</t>
-    </r>
+    <t xml:space="preserve">US$43.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$58.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Discount - Volume Discount:USAGE_BASED</t>
   </si>
   <si>
     <t xml:space="preserve">US$79.00</t>
@@ -196,25 +178,7 @@
     <t xml:space="preserve">US$95.90</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Volume Discount%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Volume Discount%:USAGE_BASED</t>
-    </r>
+    <t xml:space="preserve">Volume Discount% - Volume Discount%:USAGE_BASED</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>
@@ -252,7 +216,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -283,12 +247,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -332,7 +290,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,10 +308,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -648,8 +602,8 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -707,7 +661,7 @@
       <c r="L1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="1" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>